<commit_message>
need to do ease of review but then complete with complexity
</commit_message>
<xml_diff>
--- a/Data/cw_graded.xlsx
+++ b/Data/cw_graded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999FE848-060B-4527-9888-95FC7637B603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B1F9C-48DC-456C-980B-A9C2D5E605E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
   <dimension ref="A1:E1601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A784" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C802" sqref="C802"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +493,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -507,6 +510,9 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -521,6 +527,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -535,6 +544,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -549,6 +561,9 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -563,6 +578,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -577,6 +595,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -591,6 +612,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -604,6 +628,9 @@
       </c>
       <c r="D10">
         <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>